<commit_message>
Calculate and plot scores
</commit_message>
<xml_diff>
--- a/data/clean/input_data.xlsx
+++ b/data/clean/input_data.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,11 +618,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Allegro</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -632,32 +632,50 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>0.8</v>
+      </c>
       <c r="J3" t="n">
-        <v>2021</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>2019</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2030</v>
+      </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>189087.83</v>
-      </c>
+      <c r="M3" t="n">
+        <v>1010414</v>
+      </c>
+      <c r="N3" t="n">
+        <v>87984.8</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>https://about.allegro.eu/static-files/39ad8578-b042-4efd-a242-fa556f742a02</t>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
         </is>
       </c>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
     </row>
@@ -678,33 +696,29 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
       <c r="I4" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="J4" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K4" t="n">
         <v>2030</v>
       </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>1010414</v>
-      </c>
-      <c r="N4" t="n">
-        <v>87984.8</v>
-      </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>116611</v>
+      </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
@@ -716,23 +730,23 @@
           <t>https://corporate.ccc.eu/raporty-csr</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>dane za 2021</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>KGHM</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -742,57 +756,67 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J5" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K5" t="n">
         <v>2030</v>
       </c>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
-        <v>116611</v>
-      </c>
+      <c r="M5" t="n">
+        <v>1413129</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1614949</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
+          <t>https://kghm.com/pl/polityka-klimatyczna</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>https://corporate.ccc.eu/raporty-csr</t>
+          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>dane za 2021</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr"/>
+          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
+"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
+a także wynikające z realizacji usług czy podróży służbowych."</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KGHM</t>
+          <t>mBank</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -813,7 +837,7 @@
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>0.3</v>
+        <v>0.95</v>
       </c>
       <c r="J6" t="n">
         <v>2020</v>
@@ -823,30 +847,24 @@
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>1413129</v>
+        <v>1929.77</v>
       </c>
       <c r="N6" t="n">
-        <v>1614949</v>
+        <v>7441.65</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>https://kghm.com/pl/polityka-klimatyczna</t>
+          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
-"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
-a także wynikające z realizacji usług czy podróży służbowych."</t>
-        </is>
-      </c>
+          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
@@ -858,11 +876,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mBank</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -883,37 +901,41 @@
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="J7" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="K7" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>1929.77</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7441.65</v>
-      </c>
+        <v>505000</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0.41</v>
+      </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
+          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr"/>
+          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>bez rozbicia na Scope1 i 2</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Brak danych</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -922,11 +944,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Pekao</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -947,41 +969,41 @@
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>0.65</v>
+        <v>0.95</v>
       </c>
       <c r="J8" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="K8" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>505000</v>
-      </c>
-      <c r="N8" t="inlineStr"/>
+        <v>7380</v>
+      </c>
+      <c r="N8" t="n">
+        <v>62633</v>
+      </c>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
-        <v>0.41</v>
-      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
+          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
+          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>bez rozbicia na Scope1 i 2</t>
+          <t>scope 3 nieraportowany</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>Uwzględniane ("GC")</t>
         </is>
       </c>
       <c r="U8" t="inlineStr"/>
@@ -990,11 +1012,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>PGE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1004,7 +1026,7 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>S1+S3</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1015,34 +1037,52 @@
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>0.65</v>
+        <v>0.95</v>
       </c>
       <c r="J9" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="K9" t="n">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>72504413</v>
+      </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>scope 1 i 2 raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="T9" t="n">
+        <v>12985648</v>
+      </c>
+      <c r="U9" t="n">
+        <v>59518765000</v>
+      </c>
       <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pekao</t>
+          <t>PKN Orlen</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1066,38 +1106,36 @@
         <v>0.95</v>
       </c>
       <c r="J10" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K10" t="n">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>7380</v>
-      </c>
-      <c r="N10" t="n">
-        <v>62633</v>
-      </c>
+        <v>17307889</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
+          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/odpowiedzialnosc-za-klimat/</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
+          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
+          <t>scope 1 i 2 raportowane łącznie</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>Uwzględniane ("GC")</t>
+          <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
       <c r="U10" t="inlineStr"/>
@@ -1106,11 +1144,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PGE</t>
+          <t>PKO BP</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1131,52 +1169,54 @@
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="J11" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K11" t="n">
-        <v>2050</v>
+        <v>2025</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>72504413</v>
-      </c>
-      <c r="N11" t="inlineStr"/>
+        <v>11816</v>
+      </c>
+      <c r="N11" t="n">
+        <v>88906</v>
+      </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
+          <t>https://media.pkobp.pl/148960-pko-bank-polski-uwzglednil-wskazniki-esg-w-celach-niefinansowych</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
+          <t>https://www.raportroczny2020.pkobp.pl/esg/srodowisko/</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T11" t="n">
-        <v>12985648</v>
-      </c>
-      <c r="U11" t="n">
-        <v>59518765000</v>
-      </c>
+          <t>scope 3 usunięty</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PKN Orlen</t>
+          <t>PZU</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1186,7 +1226,7 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1195,7 +1235,9 @@
       <c r="G12" t="n">
         <v>1</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" t="n">
         <v>0.95</v>
       </c>
@@ -1203,28 +1245,32 @@
         <v>2020</v>
       </c>
       <c r="K12" t="n">
-        <v>2050</v>
+        <v>2024</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>17307889</v>
-      </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+        <v>25793</v>
+      </c>
+      <c r="N12" t="n">
+        <v>79790</v>
+      </c>
+      <c r="O12" t="n">
+        <v>18102</v>
+      </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/odpowiedzialnosc-za-klimat/</t>
+          <t>https://www.pzu.pl/relacje-inwestorskie/o-grupie/strategia</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/</t>
+          <t>https://raportroczny2020.pzu.pl/sites/pzuar19/files/download-center/raport_niefinansowy_grupy_pzu_i_pzu_sa_2020_1.pdf</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
+          <t>Scope 3 - więcej niż podróże, ale wciąż nie są to dane dot. portfela</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -1233,16 +1279,20 @@
         </is>
       </c>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PKO BP</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1252,7 +1302,7 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1261,43 +1311,45 @@
       <c r="G13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
       <c r="I13" t="n">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="J13" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K13" t="n">
-        <v>2025</v>
+        <v>2050</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>11816</v>
+        <v>4394.99</v>
       </c>
       <c r="N13" t="n">
-        <v>88906</v>
+        <v>5413.23</v>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://media.pkobp.pl/148960-pko-bank-polski-uwzglednil-wskazniki-esg-w-celach-niefinansowych</t>
+          <t>https://esg.santander.pl/2020/raport-2020/klimat/nasze-podejscie/</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>https://www.raportroczny2020.pkobp.pl/esg/srodowisko/</t>
+          <t>https://esg.santander.pl/2020/raport-2020/klimat/wplyw-na-klimat/nasz-slad-srodowiskowy/</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>scope 3 usunięty</t>
+          <t>Scope 3 obejmujący głównie podróże, plus powinien być w scope 2</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Brak danych</t>
         </is>
       </c>
       <c r="U13" t="inlineStr"/>
@@ -1306,11 +1358,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PZU</t>
+          <t>Ciech</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1320,7 +1372,7 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>S1+S2+S3</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1329,64 +1381,56 @@
       <c r="G14" t="n">
         <v>1</v>
       </c>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>0.95</v>
+        <v>0.33</v>
       </c>
       <c r="J14" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K14" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>25793</v>
+        <v>2852457</v>
       </c>
       <c r="N14" t="n">
-        <v>79790</v>
-      </c>
-      <c r="O14" t="n">
-        <v>18102</v>
-      </c>
+        <v>597284</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>https://www.pzu.pl/relacje-inwestorskie/o-grupie/strategia</t>
+          <t>https://ciechgroup.com/grupa-ciech/aktualnosci/news/grupa-ciech-przystapi-do-inicjatywy-science-based-targets-wspierajacej-firmy-w-wyznaczaniu-celow/</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>https://raportroczny2020.pzu.pl/sites/pzuar19/files/download-center/raport_niefinansowy_grupy_pzu_i_pzu_sa_2020_1.pdf</t>
+          <t>https://esgciech.com/wp-content/uploads/2021/05/Raport-niefinansowy-CIECH.pdf</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Scope 3 - więcej niż podróże, ale wciąż nie są to dane dot. portfela</t>
+          <t>scope 3 nieraportowany</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Brak danych</t>
         </is>
       </c>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Enea</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1396,7 +1440,7 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>S1+S2+S3</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1405,9 +1449,7 @@
       <c r="G15" t="n">
         <v>1</v>
       </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>0.95</v>
       </c>
@@ -1419,26 +1461,24 @@
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>4394.99</v>
-      </c>
-      <c r="N15" t="n">
-        <v>5413.23</v>
-      </c>
+        <v>18671299</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>https://esg.santander.pl/2020/raport-2020/klimat/nasze-podejscie/</t>
+          <t>https://media.enea.pl/pr/714968/neutralnosc-klimatyczna-do-2050-r-enea-zaktualizowala-strategie-rozwoju-grupy</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>https://esg.santander.pl/2020/raport-2020/klimat/wplyw-na-klimat/nasz-slad-srodowiskowy/</t>
+          <t>https://raportesg2020.csr.enea.pl/srodowisko/ograniczanie-emisji-co2/</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Scope 3 obejmujący głównie podróże, plus powinien być w scope 2</t>
+          <t>emisje raportowane łącznie</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -1452,11 +1492,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ciech</t>
+          <t>GPW</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1477,31 +1517,31 @@
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J16" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="K16" t="n">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>2852457</v>
+        <v>97.70999999999999</v>
       </c>
       <c r="N16" t="n">
-        <v>597284</v>
+        <v>3382.76</v>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>https://ciechgroup.com/grupa-ciech/aktualnosci/news/grupa-ciech-przystapi-do-inicjatywy-science-based-targets-wspierajacej-firmy-w-wyznaczaniu-celow/</t>
+          <t>https://www.gpw.pl/pub/GPW/ESG/Strategia_ESG_Grupy_Kapitalowej_GPW.pdf</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>https://esgciech.com/wp-content/uploads/2021/05/Raport-niefinansowy-CIECH.pdf</t>
+          <t>https://www.gpw.pl/pub/GPW/files/raporty_roczne/GPW_Raport_21.pdf</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1511,20 +1551,24 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
       <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Enea</t>
+          <t>Grupa Azoty</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1540,57 +1584,53 @@
       <c r="F17" t="n">
         <v>1</v>
       </c>
-      <c r="G17" t="n">
-        <v>1</v>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>0.95</v>
+        <v>0.34</v>
       </c>
       <c r="J17" t="n">
         <v>2020</v>
       </c>
       <c r="K17" t="n">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>18671299</v>
-      </c>
-      <c r="N17" t="inlineStr"/>
+        <v>7326000</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2036000</v>
+      </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://media.enea.pl/pr/714968/neutralnosc-klimatyczna-do-2050-r-enea-zaktualizowala-strategie-rozwoju-grupy</t>
+          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>https://raportesg2020.csr.enea.pl/srodowisko/ograniczanie-emisji-co2/</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>emisje raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>Brak danych</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr"/>
+          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>306381</v>
+      </c>
+      <c r="U17" t="n">
+        <v>6916601</v>
+      </c>
       <c r="V17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GPW</t>
+          <t>Grupa Azoty</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1600,42 +1640,40 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>1</v>
-      </c>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>1</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="J18" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="K18" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>97.70999999999999</v>
+        <v>7326000</v>
       </c>
       <c r="N18" t="n">
-        <v>3382.76</v>
+        <v>2036000</v>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>https://www.gpw.pl/pub/GPW/ESG/Strategia_ESG_Grupy_Kapitalowej_GPW.pdf</t>
+          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>https://www.gpw.pl/pub/GPW/files/raporty_roczne/GPW_Raport_21.pdf</t>
+          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -1643,26 +1681,18 @@
           <t>scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Grupa Azoty</t>
+          <t>ING</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1672,57 +1702,65 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">S1 </t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>0.34</v>
+        <v>0.95</v>
       </c>
       <c r="J19" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K19" t="n">
         <v>2030</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>7326000</v>
-      </c>
-      <c r="N19" t="inlineStr"/>
+        <v>5271.27</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1506687</v>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+          <t>https://www.ing.pl/_fileserver/item/1128229</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="n">
-        <v>306381</v>
-      </c>
-      <c r="U19" t="n">
-        <v>6916601</v>
-      </c>
+          <t>https://www.ing.pl/_fileserver/item/t1kv0qw</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Scope 3 obejmuje tylko podróże służbowe, nie uwzględniałem</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Grupa Azoty</t>
+          <t>Tauron</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1732,10 +1770,12 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
       <c r="G20" t="n">
         <v>1</v>
       </c>
@@ -1744,45 +1784,49 @@
         <v>0.51</v>
       </c>
       <c r="J20" t="n">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="K20" t="n">
         <v>2030</v>
       </c>
       <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="n">
-        <v>2036000</v>
-      </c>
+      <c r="M20" t="n">
+        <v>18441041.57</v>
+      </c>
+      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+          <t>https://raport.tauron.pl/zrownowazony-rozwoj/srodowisko-naturalne-i-klimat/polityka-klimatyczna-grupy-tauron/</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
+          <t>https://raport2019.tauron.pl/wp-content/uploads/2020/04/Podpisane_Sprawozdanie-na-temat-informacji-niefinansowych-GT-z-2019-rok_.pdf</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+          <t>emisje raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="T20" t="n">
+        <v>3811319574</v>
+      </c>
+      <c r="U20" t="n">
+        <v>14629722000</v>
+      </c>
       <c r="V20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ING</t>
+          <t>Wirtualna Polska</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1803,36 +1847,36 @@
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
       <c r="J21" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K21" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>5271.27</v>
+        <v>405.5</v>
       </c>
       <c r="N21" t="n">
-        <v>1506687</v>
+        <v>443.9</v>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>https://www.ing.pl/_fileserver/item/1128229</t>
+          <t>https://holding.wpcdn.pl/download/ESG%20Strategy_Wirtualna%20Polska%20Holding_2022.pdf</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>https://www.ing.pl/_fileserver/item/t1kv0qw</t>
+          <t>https://holding.wpcdn.pl/download/WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf?title=WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf&amp;button=Pobierz</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Scope 3 obejmuje tylko podróże służbowe, nie uwzględniałem</t>
+          <t>scope 3 nieraportowany</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -1846,11 +1890,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tauron</t>
+          <t>BNP Paribas</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1860,7 +1904,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1869,54 +1913,62 @@
       <c r="G22" t="n">
         <v>1</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
       <c r="I22" t="n">
-        <v>0.51</v>
+        <v>0.55</v>
       </c>
       <c r="J22" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="K22" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>18441041.57</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
+        <v>6094</v>
+      </c>
+      <c r="N22" t="n">
+        <v>12890</v>
+      </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>https://raport.tauron.pl/zrownowazony-rozwoj/srodowisko-naturalne-i-klimat/polityka-klimatyczna-grupy-tauron/</t>
+          <t>https://www.bnpparibas.pl/relacje-inwestorskie/o-banku/strategia-banku</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>https://raport2019.tauron.pl/wp-content/uploads/2020/04/Podpisane_Sprawozdanie-na-temat-informacji-niefinansowych-GT-z-2019-rok_.pdf</t>
+          <t>https://raportroczny.bnpparibas.pl/2020/</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>emisje raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T22" t="n">
-        <v>3811319574</v>
-      </c>
-      <c r="U22" t="n">
-        <v>14629722000</v>
-      </c>
-      <c r="V22" t="inlineStr"/>
+          <t>Scope 3 obejmuje podróże służbowe, tylko, do usunięcia imo</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Wirtualna Polska</t>
+          <t>Bank Ochrony Środowiska</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1926,7 +1978,7 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1935,38 +1987,40 @@
       <c r="G23" t="n">
         <v>1</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
       <c r="I23" t="n">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="J23" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K23" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>405.5</v>
+        <v>14</v>
       </c>
       <c r="N23" t="n">
-        <v>443.9</v>
+        <v>3040.78</v>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>https://holding.wpcdn.pl/download/ESG%20Strategy_Wirtualna%20Polska%20Holding_2022.pdf</t>
+          <t>https://www.bosbank.pl/__data/assets/pdf_file/0013/40333/Polityka-klimatyczna.pdf</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>https://holding.wpcdn.pl/download/WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf?title=WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf&amp;button=Pobierz</t>
+          <t>https://www.bosbank.pl/__data/assets/pdf_file/0017/40337/RAPORT-ESG-BOS.pdf</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
+          <t>Scope 3 obejmuje głównie podróże służbowe</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
@@ -1976,320 +2030,6 @@
       </c>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>BNP Paribas</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>19</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Absolute</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>S1+S2+S3</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J24" t="n">
-        <v>2019</v>
-      </c>
-      <c r="K24" t="n">
-        <v>2025</v>
-      </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
-        <v>6094</v>
-      </c>
-      <c r="N24" t="n">
-        <v>12890</v>
-      </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>https://www.bnpparibas.pl/relacje-inwestorskie/o-banku/strategia-banku</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>https://raportroczny.bnpparibas.pl/2020/</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>Scope 3 obejmuje podróże służbowe, tylko, do usunięcia imo</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Bank Ochrony Środowiska</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>20</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Absolute</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>S1+S2+S3</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="J25" t="n">
-        <v>2020</v>
-      </c>
-      <c r="K25" t="n">
-        <v>2030</v>
-      </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
-        <v>14</v>
-      </c>
-      <c r="N25" t="n">
-        <v>3040.78</v>
-      </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>https://www.bosbank.pl/__data/assets/pdf_file/0013/40333/Polityka-klimatyczna.pdf</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>https://www.bosbank.pl/__data/assets/pdf_file/0017/40337/RAPORT-ESG-BOS.pdf</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>Scope 3 obejmuje głównie podróże służbowe</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>JSW</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>21</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Absolute</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J26" t="n">
-        <v>2018</v>
-      </c>
-      <c r="K26" t="n">
-        <v>2030</v>
-      </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
-        <v>7170000</v>
-      </c>
-      <c r="N26" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>https://www.jsw.pl/relacje-inwestorskie/strategia</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>https://www.jsw.pl/raportroczny-2021/zrownowazony-rozwoj-w-jsw/w-trosce-o-klimat</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>Scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Grupa Kęty</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>22</v>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>https://grupakety.com/zrownowazony-rozwoj/srodowisko/polityka-srodowiskowa/</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Eurocash</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>23</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Absolute</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="n">
-        <v>2030</v>
-      </c>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>https://grupaeurocash.pl/assets/media/strategia-2023-2025-pl.pdf</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>https://grupaeurocash.pl/assets/media/eurocash-raport-so1-2021-pl.pdf</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CitiBank Handlowy</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>24</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2302,7 +2042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3176,162 +2916,6 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>JSW</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>21</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>B051</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="n">
-        <v>6518.69</v>
-      </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Grupa Kęty</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>22</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>C2420</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="n">
-        <v>5365.48</v>
-      </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Eurocash</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>G4711</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="n">
-        <v>1889.84</v>
-      </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CitiBank Handlowy</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>24</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>K6419</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="n">
-        <v>9120.040000000001</v>
-      </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3344,7 +2928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3759,82 +3343,6 @@
       </c>
       <c r="E21" t="inlineStr"/>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>JSW</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>21</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>PLJSW0000015</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>6518.69</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Grupa Kęty</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>22</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>PLKETY000011</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>5365.48</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Eurocash</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>PLEURCH00011</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>1889.84</v>
-      </c>
-      <c r="E24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CitiBank Handlowy</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>24</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>PLBH00000012</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>9120.040000000001</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data and methodology for calculating combined S1S2S3 score
</commit_message>
<xml_diff>
--- a/data/clean/input_data.xlsx
+++ b/data/clean/input_data.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,13 +643,13 @@
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="J3" t="n">
         <v>2019</v>
       </c>
       <c r="K3" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
@@ -696,26 +696,32 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>0.4</v>
       </c>
       <c r="J4" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="K4" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>4295.1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>63655.6</v>
+      </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
@@ -728,23 +734,23 @@
           <t>https://corporate.ccc.eu/raporty-csr</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>dane za 2021</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KGHM</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -754,67 +760,47 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
       <c r="I5" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="J5" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K5" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>1413129</v>
+        <v>4295.1</v>
       </c>
       <c r="N5" t="n">
-        <v>1614949</v>
+        <v>63665.6</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>https://kghm.com/pl/polityka-klimatyczna</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
-"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
-a także wynikające z realizacji usług czy podróży służbowych."</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mBank</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -824,61 +810,47 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
       <c r="I6" t="n">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="J6" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K6" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>1929.77</v>
+        <v>4295.1</v>
       </c>
       <c r="N6" t="n">
-        <v>7441.65</v>
+        <v>63655.6</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
-        </is>
-      </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -899,54 +871,38 @@
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="J7" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="K7" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>505000</v>
-      </c>
-      <c r="N7" t="inlineStr"/>
+        <v>4295.1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>63665.6</v>
+      </c>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>bez rozbicia na Scope1 i 2</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>Brak danych</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -956,7 +912,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>S1+S2+S3</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -965,23 +921,23 @@
       <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="J8" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="K8" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>505000</v>
-      </c>
-      <c r="N8" t="inlineStr"/>
+        <v>4295.1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>63655.6</v>
+      </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -994,11 +950,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pekao</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1008,65 +964,59 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
       <c r="I9" t="n">
-        <v>0.95</v>
+        <v>0.4</v>
       </c>
       <c r="J9" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="K9" t="n">
         <v>2030</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>7380</v>
+        <v>4295.1</v>
       </c>
       <c r="N9" t="n">
-        <v>62633</v>
+        <v>63665.6</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>Uwzględniane ("GC")</t>
-        </is>
-      </c>
+          <t>dane za 2021</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PGE</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1076,63 +1026,59 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
       <c r="I10" t="n">
-        <v>0.95</v>
+        <v>0.4</v>
       </c>
       <c r="J10" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K10" t="n">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>72504413</v>
-      </c>
-      <c r="N10" t="inlineStr"/>
+        <v>4295.1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>63655.6</v>
+      </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T10" t="n">
-        <v>12985648</v>
-      </c>
-      <c r="U10" t="n">
-        <v>59518765000</v>
-      </c>
+          <t>dane za 2021</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PKN Orlen</t>
+          <t>KGHM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1153,36 +1099,38 @@
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>0.95</v>
+        <v>0.3</v>
       </c>
       <c r="J11" t="n">
         <v>2020</v>
       </c>
       <c r="K11" t="n">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>17715216</v>
+        <v>1430234</v>
       </c>
       <c r="N11" t="n">
-        <v>1259736</v>
+        <v>1614949</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/odpowiedzialnosc-za-klimat/</t>
+          <t>https://kghm.com/pl/polityka-klimatyczna</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/ oraz https://www.orlen.pl/content/dam/internet/orlen/pl/pl/o-firmie/zrownowazony-rozwoj/emisje-grupy-orlen/Emisje%20Grupy%20ORLEN%20za%20lata%202019-2021%20-%20PL.pdf.coredownload.pdf </t>
+          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
+          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
+"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
+a także wynikające z realizacji usług czy podróży służbowych."</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -1191,20 +1139,16 @@
         </is>
       </c>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PKO BP</t>
+          <t>KGHM</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1225,58 +1169,38 @@
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="J12" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K12" t="n">
-        <v>2025</v>
+        <v>2050</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>11816</v>
+        <v>1430234</v>
       </c>
       <c r="N12" t="n">
-        <v>88906</v>
+        <v>1614949</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>https://media.pkobp.pl/148960-pko-bank-polski-uwzglednil-wskazniki-esg-w-celach-niefinansowych</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>https://www.raportroczny2020.pkobp.pl/esg/srodowisko/</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>scope 3 usunięty</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PZU</t>
+          <t>mBank</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1303,52 +1227,44 @@
         <v>2020</v>
       </c>
       <c r="K13" t="n">
-        <v>2024</v>
+        <v>2030</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>25793</v>
+        <v>1929.77</v>
       </c>
       <c r="N13" t="n">
-        <v>79790</v>
+        <v>7441.65</v>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://www.pzu.pl/relacje-inwestorskie/o-grupie/strategia</t>
+          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>https://raportroczny2020.pzu.pl/sites/pzuar19/files/download-center/raport_niefinansowy_grupy_pzu_i_pzu_sa_2020_1.pdf</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>Scope 3 - więcej niż podróże, ale wciąż nie są to dane dot. portfela</t>
-        </is>
-      </c>
+          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
       <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>mBank</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1381,44 +1297,28 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>2031.82</v>
+        <v>1929.77</v>
       </c>
       <c r="N14" t="n">
-        <v>7676.4</v>
+        <v>7441.65</v>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>https://esg.santander.pl/2020/raport-2020/klimat/nasze-podejscie/</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>https://esg.santander.pl/2020/raport-2020/klimat/wplyw-na-klimat/nasz-slad-srodowiskowy/</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Scope 3 obejmujący głównie podróże, plus powinien być w scope 2</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Brak danych</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ciech</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1439,36 +1339,36 @@
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>0.33</v>
+        <v>0.65</v>
       </c>
       <c r="J15" t="n">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="K15" t="n">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>2852457</v>
-      </c>
-      <c r="N15" t="n">
-        <v>597284</v>
-      </c>
+        <v>505000</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>0.41</v>
+      </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>https://ciechgroup.com/grupa-ciech/aktualnosci/news/grupa-ciech-przystapi-do-inicjatywy-science-based-targets-wspierajacej-firmy-w-wyznaczaniu-celow/</t>
+          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>https://esgciech.com/wp-content/uploads/2021/05/Raport-niefinansowy-CIECH.pdf</t>
+          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
+          <t>bez rozbicia na Scope1 i 2</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -1482,11 +1382,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Enea</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1496,7 +1396,7 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1505,54 +1405,40 @@
       <c r="G16" t="n">
         <v>1</v>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" t="n">
         <v>0.95</v>
       </c>
       <c r="J16" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="K16" t="n">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>18671299</v>
+        <v>505000</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>https://media.enea.pl/pr/714968/neutralnosc-klimatyczna-do-2050-r-enea-zaktualizowala-strategie-rozwoju-grupy</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>https://raportesg2020.csr.enea.pl/srodowisko/ograniczanie-emisji-co2/</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>emisje raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Brak danych</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GPW</t>
+          <t>Pekao</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1573,31 +1459,31 @@
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="J17" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K17" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>97.70999999999999</v>
+        <v>8104.3</v>
       </c>
       <c r="N17" t="n">
-        <v>3382.76</v>
+        <v>64153.1</v>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://www.gpw.pl/pub/GPW/ESG/Strategia_ESG_Grupy_Kapitalowej_GPW.pdf</t>
+          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>https://www.gpw.pl/pub/GPW/files/raporty_roczne/GPW_Raport_21.pdf</t>
+          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -1607,24 +1493,20 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Uwzględniane ("GC")</t>
         </is>
       </c>
       <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Grupa Azoty</t>
+          <t>PGE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1634,59 +1516,63 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>0.34</v>
+        <v>0.95</v>
       </c>
       <c r="J18" t="n">
         <v>2020</v>
       </c>
       <c r="K18" t="n">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>7326000</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2036000</v>
-      </c>
+        <v>72504413</v>
+      </c>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr"/>
+          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>scope 1 i 2 raportowane łącznie</t>
+        </is>
+      </c>
       <c r="T18" t="n">
-        <v>306381</v>
+        <v>12985648</v>
       </c>
       <c r="U18" t="n">
-        <v>6916601</v>
+        <v>59518765000</v>
       </c>
       <c r="V18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Grupa Azoty</t>
+          <t>PKN Orlen</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1696,59 +1582,69 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
       <c r="G19" t="n">
         <v>1</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>0.51</v>
+        <v>0.95</v>
       </c>
       <c r="J19" t="n">
         <v>2020</v>
       </c>
       <c r="K19" t="n">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>7326000</v>
+        <v>17715216</v>
       </c>
       <c r="N19" t="n">
-        <v>2036000</v>
+        <v>1259736</v>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/odpowiedzialnosc-za-klimat/</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
+          <t xml:space="preserve">https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/ oraz https://www.orlen.pl/content/dam/internet/orlen/pl/pl/o-firmie/zrownowazony-rozwoj/emisje-grupy-orlen/Emisje%20Grupy%20ORLEN%20za%20lata%202019-2021%20-%20PL.pdf.coredownload.pdf </t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr"/>
+          <t>scope 1 i 2 raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
       <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ING</t>
+          <t>PKO BP</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1769,36 +1665,36 @@
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="J20" t="n">
         <v>2019</v>
       </c>
       <c r="K20" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>5271.27</v>
+        <v>11816</v>
       </c>
       <c r="N20" t="n">
-        <v>1506687</v>
+        <v>88906</v>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>https://www.ing.pl/_fileserver/item/1128229</t>
+          <t>https://media.pkobp.pl/148960-pko-bank-polski-uwzglednil-wskazniki-esg-w-celach-niefinansowych</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>https://www.ing.pl/_fileserver/item/t1kv0qw</t>
+          <t>https://www.raportroczny2020.pkobp.pl/esg/srodowisko/</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Scope 3 obejmuje tylko podróże służbowe, nie uwzględniałem</t>
+          <t>scope 3 usunięty</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
@@ -1807,16 +1703,20 @@
         </is>
       </c>
       <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tauron</t>
+          <t>PZU</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1837,52 +1737,58 @@
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>0.51</v>
+        <v>0.95</v>
       </c>
       <c r="J21" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="K21" t="n">
-        <v>2030</v>
+        <v>2024</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>18441041.57</v>
-      </c>
-      <c r="N21" t="inlineStr"/>
+        <v>25793</v>
+      </c>
+      <c r="N21" t="n">
+        <v>79790</v>
+      </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>https://raport.tauron.pl/zrownowazony-rozwoj/srodowisko-naturalne-i-klimat/polityka-klimatyczna-grupy-tauron/</t>
+          <t>https://www.pzu.pl/relacje-inwestorskie/o-grupie/strategia</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>https://raport2019.tauron.pl/wp-content/uploads/2020/04/Podpisane_Sprawozdanie-na-temat-informacji-niefinansowych-GT-z-2019-rok_.pdf</t>
+          <t>https://raportroczny2020.pzu.pl/sites/pzuar19/files/download-center/raport_niefinansowy_grupy_pzu_i_pzu_sa_2020_1.pdf</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>emisje raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v>3811319574</v>
-      </c>
-      <c r="U21" t="n">
-        <v>14629722000</v>
-      </c>
-      <c r="V21" t="inlineStr"/>
+          <t>Scope 3 - więcej niż podróże, ale wciąż nie są to dane dot. portfela</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Wirtualna Polska</t>
+          <t>PZU</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1892,7 +1798,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1901,56 +1807,42 @@
       <c r="G22" t="n">
         <v>1</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
       <c r="I22" t="n">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="J22" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K22" t="n">
-        <v>2025</v>
+        <v>2050</v>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>405.5</v>
+        <v>25793</v>
       </c>
       <c r="N22" t="n">
-        <v>443.9</v>
+        <v>79790</v>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>https://holding.wpcdn.pl/download/ESG%20Strategy_Wirtualna%20Polska%20Holding_2022.pdf</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>https://holding.wpcdn.pl/download/WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf?title=WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf&amp;button=Pobierz</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BNP Paribas</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1973,58 +1865,54 @@
         <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="J23" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K23" t="n">
-        <v>2025</v>
+        <v>2050</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>6094</v>
+        <v>2031.82</v>
       </c>
       <c r="N23" t="n">
-        <v>12890</v>
+        <v>7676.4</v>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>https://www.bnpparibas.pl/relacje-inwestorskie/o-banku/strategia-banku</t>
+          <t>https://esg.santander.pl/2020/raport-2020/klimat/nasze-podejscie/</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>https://raportroczny.bnpparibas.pl/2020/</t>
+          <t>https://esg.santander.pl/2020/raport-2020/klimat/wplyw-na-klimat/nasz-slad-srodowiskowy/</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Scope 3 obejmuje podróże służbowe, tylko, do usunięcia imo</t>
+          <t>Scope 3 obejmujący głównie podróże, plus powinien być w scope 2</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Brak danych</t>
         </is>
       </c>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bank Ochrony Środowiska</t>
+          <t>Ciech</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -2034,7 +1922,7 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>S1+S2+S3</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -2043,45 +1931,43 @@
       <c r="G24" t="n">
         <v>1</v>
       </c>
-      <c r="H24" t="n">
-        <v>1</v>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>0.95</v>
+        <v>0.33</v>
       </c>
       <c r="J24" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K24" t="n">
-        <v>2030</v>
+        <v>2026</v>
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>14</v>
+        <v>2852457</v>
       </c>
       <c r="N24" t="n">
-        <v>3040.78</v>
+        <v>597284</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>https://www.bosbank.pl/__data/assets/pdf_file/0013/40333/Polityka-klimatyczna.pdf</t>
+          <t>https://ciechgroup.com/grupa-ciech/aktualnosci/news/grupa-ciech-przystapi-do-inicjatywy-science-based-targets-wspierajacej-firmy-w-wyznaczaniu-celow/</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>https://www.bosbank.pl/__data/assets/pdf_file/0017/40337/RAPORT-ESG-BOS.pdf</t>
+          <t>https://esgciech.com/wp-content/uploads/2021/05/Raport-niefinansowy-CIECH.pdf</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Scope 3 obejmuje głównie podróże służbowe</t>
+          <t>scope 3 nieraportowany</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
+          <t>Brak danych</t>
         </is>
       </c>
       <c r="U24" t="inlineStr"/>
@@ -2090,11 +1976,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>JSW</t>
+          <t>Ciech</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2115,64 +2001,48 @@
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>0.3</v>
+        <v>0.95</v>
       </c>
       <c r="J25" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="K25" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>7170000</v>
+        <v>2852457</v>
       </c>
       <c r="N25" t="n">
-        <v>1050000</v>
+        <v>597284</v>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>https://www.jsw.pl/relacje-inwestorskie/strategia</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>https://www.jsw.pl/raportroczny-2021/zrownowazony-rozwoj-w-jsw/w-trosce-o-klimat</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>Scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Grupa Kęty</t>
+          <t>Enea</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Intensity</t>
+          <t>Absolute</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -2183,48 +2053,52 @@
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>0.15</v>
+        <v>0.95</v>
       </c>
       <c r="J26" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="K26" t="n">
-        <v>2025</v>
+        <v>2050</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>21123</v>
+        <v>18671299</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>https://grupakety.com/zrownowazony-rozwoj/srodowisko/polityka-srodowiskowa/</t>
+          <t>https://media.enea.pl/pr/714968/neutralnosc-klimatyczna-do-2050-r-enea-zaktualizowala-strategie-rozwoju-grupy</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>https://grupakety.com/wp-content/uploads/2021/11/raport2016pl.pdf</t>
+          <t>https://raportesg2020.csr.enea.pl/srodowisko/ograniczanie-emisji-co2/</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Target: obniżenie o 15% ghg przypadających na jednostkę produktu</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr"/>
+          <t>emisje raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Brak danych</t>
+        </is>
+      </c>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Eurocash</t>
+          <t>GPW</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -2245,50 +2119,58 @@
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>0.42</v>
+        <v>0.5</v>
       </c>
       <c r="J27" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="K27" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>37825.8</v>
+        <v>97.70999999999999</v>
       </c>
       <c r="N27" t="n">
-        <v>106461.65</v>
+        <v>3382.76</v>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>https://grupaeurocash.pl/assets/media/strategia-2023-2025-pl.pdf</t>
+          <t>https://www.gpw.pl/pub/GPW/ESG/Strategia_ESG_Grupy_Kapitalowej_GPW.pdf</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>https://grupaeurocash.pl/assets/media/eurocash-raport-so1-2021-pl.pdf</t>
+          <t>https://www.gpw.pl/pub/GPW/files/raporty_roczne/GPW_Raport_21.pdf</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Scope 3 nieraportowany</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr"/>
+          <t>scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
       <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CitiBank Handlowy</t>
+          <t>GPW</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -2309,45 +2191,815 @@
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="J28" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="K28" t="n">
-        <v>2024</v>
+        <v>2030</v>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>1937</v>
+        <v>97.70999999999999</v>
       </c>
       <c r="N28" t="n">
-        <v>16337</v>
+        <v>3382.76</v>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>https://www.citibank.pl/poland/homepage/polish/press1/files/220217-1_ip.pdf</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>https://www.citibank.pl/poland/homepage/raport_roczny_2019/files/sprawozdanie_na_temat_informacji_niefinansowych_2019_pl.pdf</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>Brak celow dla Scope 3</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Grupa Azoty</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>15</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K29" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="n">
+        <v>7326000</v>
+      </c>
+      <c r="N29" t="n">
+        <v>2036000</v>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="n">
+        <v>306381</v>
+      </c>
+      <c r="U29" t="n">
+        <v>6916601</v>
+      </c>
+      <c r="V29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Grupa Azoty</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K30" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="n">
+        <v>7326000</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2036000</v>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ING</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>16</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K31" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="n">
+        <v>5271.27</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1506687</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>https://www.ing.pl/_fileserver/item/1128229</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>https://www.ing.pl/_fileserver/item/t1kv0qw</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>Scope 3 obejmuje tylko podróże służbowe, nie uwzględniałem</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Tauron</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>17</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2018</v>
+      </c>
+      <c r="K32" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>https://raport.tauron.pl/zrownowazony-rozwoj/srodowisko-naturalne-i-klimat/polityka-klimatyczna-grupy-tauron/</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>https://raport2019.tauron.pl/wp-content/uploads/2020/04/Podpisane_Sprawozdanie-na-temat-informacji-niefinansowych-GT-z-2019-rok_.pdf</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>emisje raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="T32" t="n">
+        <v>3811319574</v>
+      </c>
+      <c r="U32" t="n">
+        <v>14629722000</v>
+      </c>
+      <c r="V32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Wirtualna Polska</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>18</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2021</v>
+      </c>
+      <c r="K33" t="n">
+        <v>2025</v>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="n">
+        <v>405.5</v>
+      </c>
+      <c r="N33" t="n">
+        <v>443.9</v>
+      </c>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>https://holding.wpcdn.pl/download/ESG%20Strategy_Wirtualna%20Polska%20Holding_2022.pdf</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>https://holding.wpcdn.pl/download/WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf?title=WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf&amp;button=Pobierz</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Wirtualna Polska</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>18</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2021</v>
+      </c>
+      <c r="K34" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="n">
+        <v>405.5</v>
+      </c>
+      <c r="N34" t="n">
+        <v>443.9</v>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BNP Paribas</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>19</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>S1+S2+S3</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2025</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="n">
+        <v>6094</v>
+      </c>
+      <c r="N35" t="n">
+        <v>12890</v>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>https://www.bnpparibas.pl/relacje-inwestorskie/o-banku/strategia-banku</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>https://raportroczny.bnpparibas.pl/2020/</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>Scope 3 obejmuje podróże służbowe, tylko, do usunięcia imo</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Bank Ochrony Środowiska</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>20</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>S1+S2+S3</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="J36" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K36" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="n">
+        <v>14</v>
+      </c>
+      <c r="N36" t="n">
+        <v>3040.78</v>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>https://www.bosbank.pl/__data/assets/pdf_file/0013/40333/Polityka-klimatyczna.pdf</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>https://www.bosbank.pl/__data/assets/pdf_file/0017/40337/RAPORT-ESG-BOS.pdf</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>Scope 3 obejmuje głównie podróże służbowe</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>JSW</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>21</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2018</v>
+      </c>
+      <c r="K37" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="n">
+        <v>7170000</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>https://www.jsw.pl/relacje-inwestorskie/strategia</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>https://www.jsw.pl/raportroczny-2021/zrownowazony-rozwoj-w-jsw/w-trosce-o-klimat</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>Scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Grupa Kęty</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>22</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Intensity</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J38" t="n">
+        <v>2016</v>
+      </c>
+      <c r="K38" t="n">
+        <v>2025</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="n">
+        <v>21123</v>
+      </c>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>https://grupakety.com/zrownowazony-rozwoj/srodowisko/polityka-srodowiskowa/</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>https://grupakety.com/wp-content/uploads/2021/11/raport2016pl.pdf</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>Target: obniżenie o 15% ghg przypadających na jednostkę produktu</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Eurocash</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>23</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K39" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>37825.8</v>
+      </c>
+      <c r="N39" t="n">
+        <v>106461.65</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>https://grupaeurocash.pl/assets/media/strategia-2023-2025-pl.pdf</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>https://grupaeurocash.pl/assets/media/eurocash-raport-so1-2021-pl.pdf</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>Scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CitiBank Handlowy</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>24</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K40" t="n">
+        <v>2024</v>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="n">
+        <v>1937</v>
+      </c>
+      <c r="N40" t="n">
+        <v>16337</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>https://www.citibank.pl/poland/homepage/polish/press1/files/220217-1_ip.pdf</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>https://www.citibank.pl/poland/homepage/raport_roczny_2019/files/sprawozdanie_na_temat_informacji_niefinansowych_2019_pl.pdf</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>Brak celow dla Scope 3</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2484,18 +3136,18 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>5352870000</v>
+      </c>
       <c r="N2" t="n">
         <v>39763.72</v>
       </c>
       <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>16869877000</v>
+      </c>
       <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2527,18 +3179,18 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>5638600000</v>
+      </c>
       <c r="N3" t="n">
         <v>5788.57</v>
       </c>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>66647400000</v>
+      </c>
       <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -2570,18 +3222,18 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>29803000000</v>
+      </c>
       <c r="N4" t="n">
         <v>27880</v>
       </c>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>48027000000</v>
+      </c>
       <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -2613,18 +3265,18 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>7146633000</v>
+      </c>
       <c r="N5" t="n">
         <v>18361.13</v>
       </c>
       <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>199538885000</v>
+      </c>
       <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -2656,18 +3308,18 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>11928000000</v>
+      </c>
       <c r="N6" t="n">
         <v>11089.42</v>
       </c>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>26157000000</v>
+      </c>
       <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -2699,18 +3351,18 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>9100353000</v>
+      </c>
       <c r="N7" t="n">
         <v>32021.34</v>
       </c>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>250566605000</v>
+      </c>
       <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2742,18 +3394,18 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>52730000000</v>
+      </c>
       <c r="N8" t="n">
         <v>15074.01</v>
       </c>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>88966000000</v>
+      </c>
       <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -2785,18 +3437,18 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>131341000000</v>
+      </c>
       <c r="N9" t="n">
         <v>31795.89</v>
       </c>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>106754000000</v>
+      </c>
       <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -2828,18 +3480,18 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>10568000000</v>
+      </c>
       <c r="N10" t="n">
         <v>56162.5</v>
       </c>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>418086000000</v>
+      </c>
       <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -2871,18 +3523,18 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>7454000000</v>
+      </c>
       <c r="N11" t="n">
         <v>30525.54</v>
       </c>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>402129000000</v>
+      </c>
       <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -2914,18 +3566,18 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>9335175000</v>
+      </c>
       <c r="N12" t="n">
         <v>35612.98</v>
       </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>244876340000</v>
+      </c>
       <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -2957,18 +3609,18 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>3459915000</v>
+      </c>
       <c r="N13" t="n">
         <v>2213.4</v>
       </c>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>7145820000</v>
+      </c>
       <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -3000,18 +3652,18 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>8018616000</v>
+      </c>
       <c r="N14" t="n">
         <v>3756.68</v>
       </c>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>34627647000</v>
+      </c>
       <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -3043,18 +3695,18 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>407571000</v>
+      </c>
       <c r="N15" t="n">
         <v>1738.48</v>
       </c>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>1410688000</v>
+      </c>
       <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -3086,18 +3738,18 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="n">
+        <v>15901259000</v>
+      </c>
       <c r="N16" t="n">
         <v>3352.81</v>
       </c>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>23644705000</v>
+      </c>
       <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -3129,18 +3781,18 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="n">
+        <v>7757400000</v>
+      </c>
       <c r="N17" t="n">
         <v>34736.7</v>
       </c>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>201654200000</v>
+      </c>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3172,18 +3824,18 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>25614000000</v>
+      </c>
       <c r="N18" t="n">
         <v>4651.27</v>
       </c>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="n">
+        <v>40075000000</v>
+      </c>
       <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -3215,18 +3867,18 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>872239000</v>
+      </c>
       <c r="N19" t="n">
         <v>4123.71</v>
       </c>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>1262947000</v>
+      </c>
       <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
@@ -3258,18 +3910,18 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>4705359000</v>
+      </c>
       <c r="N20" t="n">
         <v>13453.71</v>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>131777481000</v>
+      </c>
       <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -3301,18 +3953,18 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="n">
+        <v>613972000</v>
+      </c>
       <c r="N21" t="n">
         <v>845.8200000000001</v>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>20585740000</v>
+      </c>
       <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3344,18 +3996,18 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>10629100000</v>
+      </c>
       <c r="N22" t="n">
         <v>4094.14</v>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>15961800000</v>
+      </c>
       <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -3387,18 +4039,18 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>4794250000</v>
+      </c>
       <c r="N23" t="n">
         <v>5886.59</v>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>3526815000</v>
+      </c>
       <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -3430,18 +4082,18 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="n">
+        <v>26281431000</v>
+      </c>
       <c r="N24" t="n">
         <v>1508.53</v>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>8487299000</v>
+      </c>
       <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -3473,18 +4125,18 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L25" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="n">
+        <v>1090108000</v>
+      </c>
       <c r="N25" t="n">
         <v>7708.92</v>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>61862771000</v>
+      </c>
       <c r="Q25" t="inlineStr"/>
     </row>
   </sheetData>
@@ -3547,9 +4199,7 @@
           <t>LU2237380790</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>29033.18</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -3566,9 +4216,7 @@
           <t>PLCCC0000016</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>2718.16</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -3585,9 +4233,7 @@
           <t>PLKGHM000017</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>21350</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -3604,9 +4250,7 @@
           <t>PLBRE0000012</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>9670.379999999999</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -3623,9 +4267,7 @@
           <t>PLTLKPL00017</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>8351.84</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -3642,9 +4284,7 @@
           <t>PLPEKAO00016</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>21050.1</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -3661,9 +4301,7 @@
           <t>PLPGER000010</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>21970.44</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -3680,9 +4318,7 @@
           <t>PLPKN0000018</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>30196.26</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -3699,9 +4335,7 @@
           <t>PLPKO0000016</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>33937.5</v>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -3718,9 +4352,7 @@
           <t>PLPZU0000011</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>26622.41</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -3737,9 +4369,7 @@
           <t>PLBZ00000044</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>24034.93</v>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -3756,9 +4386,7 @@
           <t>PLCIECH00018</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>1891.93</v>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -3775,9 +4403,7 @@
           <t>PLENEA000013</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>1891.93</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -3794,9 +4420,7 @@
           <t>PLGPW0000017</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>1544.57</v>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -3813,9 +4437,7 @@
           <t>PLZATRM00012</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>4146.37</v>
-      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -3832,9 +4454,7 @@
           <t>PLBSK0000017</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>21492.52</v>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3851,9 +4471,7 @@
           <t>PLTAURN00011</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>5436.41</v>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -3870,9 +4488,7 @@
           <t>PLWRTPL00027</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>3072.97</v>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
@@ -3889,9 +4505,7 @@
           <t>PLBGZ0000010</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>8147.14</v>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -3908,9 +4522,7 @@
           <t>PLBOS0000019</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>726.85</v>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3927,9 +4539,7 @@
           <t>PLJSW0000015</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>6518.69</v>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -3946,9 +4556,7 @@
           <t>PLKETY000011</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>5365.48</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -3965,9 +4573,7 @@
           <t>PLEURCH00011</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>1889.84</v>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -3984,9 +4590,7 @@
           <t>PLBH00000012</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>9120.040000000001</v>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data. Optional use of estimates. Score aggregations.
</commit_message>
<xml_diff>
--- a/data/clean/input_data.xlsx
+++ b/data/clean/input_data.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,35 +513,50 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>base_year_ghg_s1s2</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ghg_s3_factor</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>base_year_ghg_s3_estimate</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>achieved_reduction</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>source_goals</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>source_emissions</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Inne gazy</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>emisje tylko co2</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Metoda market based?</t>
         </is>
@@ -590,26 +605,37 @@
       <c r="N2" t="n">
         <v>10598.02</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>https://raportesg.allegro.pl/srodowisko-i-klimat/polityka-klimatyczna-i-cele-sbti/</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>https://about.allegro.eu/static-files/39ad8578-b042-4efd-a242-fa556f742a02</t>
-        </is>
+      <c r="O2" t="n">
+        <v>206039.04</v>
+      </c>
+      <c r="P2" t="n">
+        <v>11124.72</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>23361.912</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
+          <t>https://raportesg.allegro.pl/srodowisko-i-klimat/polityka-klimatyczna-i-cele-sbti/</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>https://about.allegro.eu/static-files/39ad8578-b042-4efd-a242-fa556f742a02</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr">
+        <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr">
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
         <is>
           <t>Wybrana</t>
         </is>
@@ -646,7 +672,7 @@
         <v>0.4</v>
       </c>
       <c r="J3" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K3" t="n">
         <v>2025</v>
@@ -659,25 +685,34 @@
         <v>63665.6</v>
       </c>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/raporty-csr</t>
-        </is>
+      <c r="P3" t="n">
+        <v>67960.7</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>142717.47</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -710,7 +745,7 @@
         <v>0.4</v>
       </c>
       <c r="J4" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K4" t="n">
         <v>2025</v>
@@ -723,25 +758,34 @@
         <v>63655.6</v>
       </c>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/raporty-csr</t>
-        </is>
+      <c r="P4" t="n">
+        <v>67960.7</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>142717.47</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -778,20 +822,21 @@
         <v>2025</v>
       </c>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>4295.1</v>
-      </c>
-      <c r="N5" t="n">
-        <v>63665.6</v>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -810,38 +855,45 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J6" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K6" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>4295.1</v>
       </c>
       <c r="N6" t="n">
-        <v>63655.6</v>
+        <v>63665.6</v>
       </c>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>67950.7</v>
+      </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -874,7 +926,7 @@
         <v>0.8</v>
       </c>
       <c r="J7" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="K7" t="n">
         <v>2030</v>
@@ -884,16 +936,21 @@
         <v>4295.1</v>
       </c>
       <c r="N7" t="n">
-        <v>63665.6</v>
+        <v>63655.6</v>
       </c>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>67950.7</v>
+      </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -912,18 +969,16 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>S1+S2</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
       <c r="I8" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="J8" t="n">
         <v>2019</v>
@@ -932,29 +987,42 @@
         <v>2030</v>
       </c>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>4295.1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>63655.6</v>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>https://corporate.ccc.eu/raporty-csr</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>dane za 2021</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>KGHM</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -964,59 +1032,76 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J9" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K9" t="n">
         <v>2030</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>4295.1</v>
+        <v>1430234</v>
       </c>
       <c r="N9" t="n">
-        <v>63665.6</v>
+        <v>1614949</v>
       </c>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/raporty-csr</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>dane za 2021</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>3045183</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="R9" t="n">
+        <v>8221994.1</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>https://kghm.com/pl/polityka-klimatyczna</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
+"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
+a także wynikające z realizacji usług czy podróży służbowych."</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>KGHM</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1026,59 +1111,54 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>0.4</v>
+        <v>0.95</v>
       </c>
       <c r="J10" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K10" t="n">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>4295.1</v>
+        <v>1430234</v>
       </c>
       <c r="N10" t="n">
-        <v>63655.6</v>
+        <v>1614949</v>
       </c>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/media/ESG-GO25-prezentacja-SHORT-WWW-FINAL-.pdf</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>https://corporate.ccc.eu/raporty-csr</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>dane za 2021</t>
-        </is>
-      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KGHM</t>
+          <t>mBank</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1099,7 +1179,7 @@
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>0.3</v>
+        <v>0.95</v>
       </c>
       <c r="J11" t="n">
         <v>2020</v>
@@ -1109,46 +1189,49 @@
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>1430234</v>
+        <v>1929.77</v>
       </c>
       <c r="N11" t="n">
-        <v>1614949</v>
+        <v>7441.65</v>
       </c>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>https://kghm.com/pl/polityka-klimatyczna</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>https://kghm.com/pl/inwestorzy/centrum-wynikow/raporty-zintegrowane</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>scope 3 zostanie udostępniony w 2024 roku i jest określany jako: 
-"emisje pośrednie w łańcuchu dostaw sprzętu, maszyn, części, materiałów eksploatacyjnych itp., 
-a także wynikające z realizacji usług czy podróży służbowych."</t>
-        </is>
-      </c>
+      <c r="P11" t="n">
+        <v>9371.42</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>108</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1012113.36</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
+          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr">
+        <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KGHM</t>
+          <t>mBank</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1158,7 +1241,7 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1+S2+S3</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1167,7 +1250,9 @@
       <c r="G12" t="n">
         <v>1</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" t="n">
         <v>0.95</v>
       </c>
@@ -1179,28 +1264,33 @@
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>1430234</v>
+        <v>1929.77</v>
       </c>
       <c r="N12" t="n">
-        <v>1614949</v>
+        <v>7441.65</v>
       </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>mBank</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1221,50 +1311,61 @@
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="J13" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="K13" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>1929.77</v>
-      </c>
-      <c r="N13" t="n">
-        <v>7441.65</v>
-      </c>
+        <v>505000</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>https://pl.media.mbank.pl/185727-mbank-pracuje-nad-dekarbonizacja-portfela-kredytowego-przystepuje-do-organizacji-pcaf</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>https://www.mbank.pl/raport-roczny/2020/wp-content/uploads/2021/07/mBank-Raport-zintegrowany-2020.pdf</t>
-        </is>
+      <c r="P13" t="n">
+        <v>505000</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1060500</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
+          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>bez rozbicia na Scope1 i 2</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Brak danych</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>mBank</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1290,35 +1391,38 @@
         <v>0.95</v>
       </c>
       <c r="J14" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="K14" t="n">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>1929.77</v>
-      </c>
-      <c r="N14" t="n">
-        <v>7441.65</v>
-      </c>
+        <v>505000</v>
+      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Pekao</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1339,54 +1443,63 @@
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>0.65</v>
+        <v>0.95</v>
       </c>
       <c r="J15" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="K15" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>505000</v>
-      </c>
-      <c r="N15" t="inlineStr"/>
+        <v>8104.3</v>
+      </c>
+      <c r="N15" t="n">
+        <v>64153.1</v>
+      </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://www.orange.pl/razemdlaplanety/redukujemy-emisje-co2 ; https://biuroprasowe.orange.pl/informacje-prasowe/orangegoesgreen-orange-polska-oglasza-swoje-cele-klimatyczne-redukcja-emisji-co2-i-wiecej-energii-ze-zrodel-odnawialnych/ </t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>http://www.raportcsropl.pl/kluczowe-dane-czyste-srodowisko.html#raport-section</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>bez rozbicia na Scope1 i 2</t>
-        </is>
-      </c>
+        <v>72257.39999999999</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>108</v>
+      </c>
+      <c r="R15" t="n">
+        <v>7803799.2</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Brak danych</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
+          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>scope 3 nieraportowany</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Uwzględniane ("GC")</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>PGE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1396,7 +1509,7 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>S1+S2+S3</t>
+          <t>S1+S2</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1405,40 +1518,63 @@
       <c r="G16" t="n">
         <v>1</v>
       </c>
-      <c r="H16" t="n">
-        <v>1</v>
-      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>0.95</v>
       </c>
       <c r="J16" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="K16" t="n">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>505000</v>
+        <v>72504413</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>72504413</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R16" t="n">
+        <v>108756619.5</v>
+      </c>
       <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>scope 1 i 2 raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="W16" t="n">
+        <v>12985648</v>
+      </c>
+      <c r="X16" t="n">
+        <v>59518765000</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Pekao</t>
+          <t>PKN Orlen</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1462,51 +1598,66 @@
         <v>0.95</v>
       </c>
       <c r="J17" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K17" t="n">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>8104.3</v>
+        <v>17715216</v>
       </c>
       <c r="N17" t="n">
-        <v>64153.1</v>
-      </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>https://media.pekao.com.pl/pr/676849/strategia-esg-banku-pekao-odpowiedzialny-bank-wspierajacy-zrownowazony-rozwoj</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>https://www.pekao.com.pl/dam/jcr:78de73cd-fcaf-4b94-81d7-7d08079e07ba/O%C5%9Bwiadczenie%20o%20danych%20niefinansowych%20Grupy%20Pekao%202021.pdf</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>scope 3 nieraportowany</t>
-        </is>
-      </c>
+        <v>1259736</v>
+      </c>
+      <c r="O17" t="n">
+        <v>81123571</v>
+      </c>
+      <c r="P17" t="n">
+        <v>18974952</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R17" t="n">
+        <v>142312140</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr">
         <is>
-          <t>Uwzględniane ("GC")</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
+          <t>https://www.orlen.pl/content/dam/internet/orlen/pl/pl/o-firmie/media/komunikaty-prasowe/dokumenty/Niskoemisyjny-ORLEN_09_09_2020.pdf.coredownload.pdf</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/ oraz https://www.orlen.pl/content/dam/internet/orlen/pl/pl/o-firmie/zrownowazony-rozwoj/emisje-grupy-orlen/Emisje%20Grupy%20ORLEN%20za%20lata%202019-2021%20-%20PL.pdf.coredownload.pdf </t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>scope 1 i 2 raportowane łącznie</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Uwzględniane (CO2e)</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>Wybrana</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PGE</t>
+          <t>PKN Orlen</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1520,50 +1671,41 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="J18" t="n">
         <v>2020</v>
       </c>
       <c r="K18" t="n">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>72504413</v>
-      </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+        <v>17715216</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1259736</v>
+      </c>
+      <c r="O18" t="n">
+        <v>81123571</v>
+      </c>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>https://www.gkpge.pl/grupa-pge/o-grupie/poznaj-strategie</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>https://raportzintegrowany2020.gkpge.pl/wp-content/uploads/2021/05/SprawozdanienatematinformacjiniefinansowychPGE.pdf#page=64</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T18" t="n">
-        <v>12985648</v>
-      </c>
-      <c r="U18" t="n">
-        <v>59518765000</v>
-      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1576,30 +1718,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Absolute</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+          <t>Intensity</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Power Generation</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>S1+S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1</v>
-      </c>
+        <v>0.49</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>0.95</v>
+        <v>0.33</v>
       </c>
       <c r="J19" t="n">
         <v>2020</v>
       </c>
       <c r="K19" t="n">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
@@ -1608,34 +1752,19 @@
       <c r="N19" t="n">
         <v>1259736</v>
       </c>
-      <c r="O19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>81123571</v>
+      </c>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/odpowiedzialnosc-za-klimat/</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://raportzintegrowany2020.orlen.pl/srodowisko-i-klimat/emisje-do-powietrza/ oraz https://www.orlen.pl/content/dam/internet/orlen/pl/pl/o-firmie/zrownowazony-rozwoj/emisje-grupy-orlen/Emisje%20Grupy%20ORLEN%20za%20lata%202019-2021%20-%20PL.pdf.coredownload.pdf </t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>scope 1 i 2 raportowane łącznie</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>Uwzględniane (CO2e)</t>
-        </is>
-      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>Wybrana</t>
-        </is>
-      </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1681,29 +1810,38 @@
         <v>88906</v>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
+      <c r="P20" t="n">
+        <v>100722</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>108</v>
+      </c>
+      <c r="R20" t="n">
+        <v>10877976</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr">
         <is>
           <t>https://media.pkobp.pl/148960-pko-bank-polski-uwzglednil-wskazniki-esg-w-celach-niefinansowych</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="U20" t="inlineStr">
         <is>
           <t>https://www.raportroczny2020.pkobp.pl/esg/srodowisko/</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="V20" t="inlineStr">
         <is>
           <t>scope 3 usunięty</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr">
+      <c r="W20" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr">
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr">
         <is>
           <t>Wybrana</t>
         </is>
@@ -1753,29 +1891,38 @@
         <v>79790</v>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr">
+      <c r="P21" t="n">
+        <v>105583</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>108</v>
+      </c>
+      <c r="R21" t="n">
+        <v>11402964</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr">
         <is>
           <t>https://www.pzu.pl/relacje-inwestorskie/o-grupie/strategia</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
+      <c r="U21" t="inlineStr">
         <is>
           <t>https://raportroczny2020.pzu.pl/sites/pzuar19/files/download-center/raport_niefinansowy_grupy_pzu_i_pzu_sa_2020_1.pdf</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
+      <c r="V21" t="inlineStr">
         <is>
           <t>Scope 3 - więcej niż podróże, ale wciąż nie są to dane dot. portfela</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr">
+      <c r="W21" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr">
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr">
         <is>
           <t>Wybrana</t>
         </is>
@@ -1827,13 +1974,18 @@
         <v>79790</v>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1881,29 +2033,38 @@
         <v>7676.4</v>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
+      <c r="P23" t="n">
+        <v>9708.219999999999</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>108</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1048487.76</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr">
         <is>
           <t>https://esg.santander.pl/2020/raport-2020/klimat/nasze-podejscie/</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="U23" t="inlineStr">
         <is>
           <t>https://esg.santander.pl/2020/raport-2020/klimat/wplyw-na-klimat/nasz-slad-srodowiskowy/</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="V23" t="inlineStr">
         <is>
           <t>Scope 3 obejmujący głównie podróże, plus powinien być w scope 2</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
+      <c r="W23" t="inlineStr">
         <is>
           <t>Brak danych</t>
         </is>
       </c>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1949,29 +2110,38 @@
         <v>597284</v>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
+      <c r="P24" t="n">
+        <v>3449741</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="R24" t="n">
+        <v>6554507.9</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr">
         <is>
           <t>https://ciechgroup.com/grupa-ciech/aktualnosci/news/grupa-ciech-przystapi-do-inicjatywy-science-based-targets-wspierajacej-firmy-w-wyznaczaniu-celow/</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr">
+      <c r="U24" t="inlineStr">
         <is>
           <t>https://esgciech.com/wp-content/uploads/2021/05/Raport-niefinansowy-CIECH.pdf</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="V24" t="inlineStr">
         <is>
           <t>scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr">
+      <c r="W24" t="inlineStr">
         <is>
           <t>Brak danych</t>
         </is>
       </c>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2017,13 +2187,18 @@
         <v>597284</v>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2048,9 +2223,7 @@
       <c r="F26" t="n">
         <v>1</v>
       </c>
-      <c r="G26" t="n">
-        <v>1</v>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>0.95</v>
@@ -2065,31 +2238,42 @@
       <c r="M26" t="n">
         <v>18671299</v>
       </c>
-      <c r="N26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>0.01</v>
+      </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr">
+      <c r="P26" t="n">
+        <v>18671299.01</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R26" t="n">
+        <v>28006948.52</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr">
         <is>
           <t>https://media.enea.pl/pr/714968/neutralnosc-klimatyczna-do-2050-r-enea-zaktualizowala-strategie-rozwoju-grupy</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
+      <c r="U26" t="inlineStr">
         <is>
           <t>https://raportesg2020.csr.enea.pl/srodowisko/ograniczanie-emisji-co2/</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
+      <c r="V26" t="inlineStr">
         <is>
           <t>emisje raportowane łącznie</t>
         </is>
       </c>
-      <c r="T26" t="inlineStr">
+      <c r="W26" t="inlineStr">
         <is>
           <t>Brak danych</t>
         </is>
       </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2135,29 +2319,38 @@
         <v>3382.76</v>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr">
+      <c r="P27" t="n">
+        <v>3480.47</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R27" t="n">
+        <v>7308.987</v>
+      </c>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr">
         <is>
           <t>https://www.gpw.pl/pub/GPW/ESG/Strategia_ESG_Grupy_Kapitalowej_GPW.pdf</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="U27" t="inlineStr">
         <is>
           <t>https://www.gpw.pl/pub/GPW/files/raporty_roczne/GPW_Raport_21.pdf</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="V27" t="inlineStr">
         <is>
           <t>scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
+      <c r="W27" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr">
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr">
         <is>
           <t>Wybrana</t>
         </is>
@@ -2207,13 +2400,18 @@
         <v>3382.76</v>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="P28" t="n">
+        <v>3480.47</v>
+      </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2257,25 +2455,34 @@
         <v>2036000</v>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr">
+      <c r="P29" t="n">
+        <v>9362000</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="R29" t="n">
+        <v>17787800</v>
+      </c>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr">
         <is>
           <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
+      <c r="U29" t="inlineStr">
         <is>
           <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="n">
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="n">
         <v>306381</v>
       </c>
-      <c r="U29" t="n">
+      <c r="X29" t="n">
         <v>6916601</v>
       </c>
-      <c r="V29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2320,24 +2527,27 @@
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr">
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr">
         <is>
           <t>https://grupaazoty.com/aktualnosci/grupa-azoty-ze-strategia-na-lata-2021-2030-i-kluczowym-projektem-zielone-azoty</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr">
+      <c r="U30" t="inlineStr">
         <is>
           <t>https://raport2020.grupaazoty.com/srodowisko/emisje-do-powietrza/</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
+      <c r="V30" t="inlineStr">
         <is>
           <t>scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2383,29 +2593,38 @@
         <v>1506687</v>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr">
+      <c r="P31" t="n">
+        <v>1511958.27</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>108</v>
+      </c>
+      <c r="R31" t="n">
+        <v>163291493.2</v>
+      </c>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr">
         <is>
           <t>https://www.ing.pl/_fileserver/item/1128229</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
+      <c r="U31" t="inlineStr">
         <is>
           <t>https://www.ing.pl/_fileserver/item/t1kv0qw</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="V31" t="inlineStr">
         <is>
           <t>Scope 3 obejmuje tylko podróże służbowe, nie uwzględniałem</t>
         </is>
       </c>
-      <c r="T31" t="inlineStr">
+      <c r="W31" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2444,32 +2663,43 @@
         <v>2030</v>
       </c>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="M32" t="n">
+        <v>18441041.57</v>
+      </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr">
+      <c r="P32" t="n">
+        <v>18441041.57</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R32" t="n">
+        <v>27661562.36</v>
+      </c>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr">
         <is>
           <t>https://raport.tauron.pl/zrownowazony-rozwoj/srodowisko-naturalne-i-klimat/polityka-klimatyczna-grupy-tauron/</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>https://raport2019.tauron.pl/wp-content/uploads/2020/04/Podpisane_Sprawozdanie-na-temat-informacji-niefinansowych-GT-z-2019-rok_.pdf</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="V32" t="inlineStr">
         <is>
           <t>emisje raportowane łącznie</t>
         </is>
       </c>
-      <c r="T32" t="n">
+      <c r="W32" t="n">
         <v>3811319574</v>
       </c>
-      <c r="U32" t="n">
+      <c r="X32" t="n">
         <v>14629722000</v>
       </c>
-      <c r="V32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2515,29 +2745,38 @@
         <v>443.9</v>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr">
+      <c r="P33" t="n">
+        <v>849.4</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1783.74</v>
+      </c>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr">
         <is>
           <t>https://holding.wpcdn.pl/download/ESG%20Strategy_Wirtualna%20Polska%20Holding_2022.pdf</t>
         </is>
       </c>
-      <c r="R33" t="inlineStr">
+      <c r="U33" t="inlineStr">
         <is>
           <t>https://holding.wpcdn.pl/download/WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf?title=WPL_RS_2021_Sprawozdanie_Zarzadu_z_dzialalnosci.pdf&amp;button=Pobierz</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
+      <c r="V33" t="inlineStr">
         <is>
           <t>scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T33" t="inlineStr">
+      <c r="W33" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2583,13 +2822,18 @@
         <v>443.9</v>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2637,29 +2881,38 @@
         <v>12890</v>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr">
+      <c r="P35" t="n">
+        <v>18984</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>108</v>
+      </c>
+      <c r="R35" t="n">
+        <v>2050272</v>
+      </c>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr">
         <is>
           <t>https://www.bnpparibas.pl/relacje-inwestorskie/o-banku/strategia-banku</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr">
+      <c r="U35" t="inlineStr">
         <is>
           <t>https://raportroczny.bnpparibas.pl/2020/</t>
         </is>
       </c>
-      <c r="S35" t="inlineStr">
+      <c r="V35" t="inlineStr">
         <is>
           <t>Scope 3 obejmuje podróże służbowe, tylko, do usunięcia imo</t>
         </is>
       </c>
-      <c r="T35" t="inlineStr">
+      <c r="W35" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U35" t="inlineStr"/>
-      <c r="V35" t="inlineStr">
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr">
         <is>
           <t>Wybrana</t>
         </is>
@@ -2711,29 +2964,38 @@
         <v>3040.78</v>
       </c>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr">
+      <c r="P36" t="n">
+        <v>3054.78</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>108</v>
+      </c>
+      <c r="R36" t="n">
+        <v>329916.24</v>
+      </c>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr">
         <is>
           <t>https://www.bosbank.pl/__data/assets/pdf_file/0013/40333/Polityka-klimatyczna.pdf</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr">
+      <c r="U36" t="inlineStr">
         <is>
           <t>https://www.bosbank.pl/__data/assets/pdf_file/0017/40337/RAPORT-ESG-BOS.pdf</t>
         </is>
       </c>
-      <c r="S36" t="inlineStr">
+      <c r="V36" t="inlineStr">
         <is>
           <t>Scope 3 obejmuje głównie podróże służbowe</t>
         </is>
       </c>
-      <c r="T36" t="inlineStr">
+      <c r="W36" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2779,29 +3041,38 @@
         <v>1050000</v>
       </c>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr">
+      <c r="P37" t="n">
+        <v>8220000</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="R37" t="n">
+        <v>22194000</v>
+      </c>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
         <is>
           <t>https://www.jsw.pl/relacje-inwestorskie/strategia</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr">
+      <c r="U37" t="inlineStr">
         <is>
           <t>https://www.jsw.pl/raportroczny-2021/zrownowazony-rozwoj-w-jsw/w-trosce-o-klimat</t>
         </is>
       </c>
-      <c r="S37" t="inlineStr">
+      <c r="V37" t="inlineStr">
         <is>
           <t>Scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr">
+      <c r="W37" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2819,7 +3090,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Product</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2849,25 +3120,30 @@
       </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr">
+      <c r="P38" t="n">
+        <v>21123</v>
+      </c>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr">
         <is>
           <t>https://grupakety.com/zrownowazony-rozwoj/srodowisko/polityka-srodowiskowa/</t>
         </is>
       </c>
-      <c r="R38" t="inlineStr">
+      <c r="U38" t="inlineStr">
         <is>
           <t>https://grupakety.com/wp-content/uploads/2021/11/raport2016pl.pdf</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
+      <c r="V38" t="inlineStr">
         <is>
           <t>Target: obniżenie o 15% ghg przypadających na jednostkę produktu</t>
         </is>
       </c>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2913,25 +3189,34 @@
         <v>106461.65</v>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr">
+      <c r="P39" t="n">
+        <v>144287.45</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>10</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1442874.5</v>
+      </c>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr">
         <is>
           <t>https://grupaeurocash.pl/assets/media/strategia-2023-2025-pl.pdf</t>
         </is>
       </c>
-      <c r="R39" t="inlineStr">
+      <c r="U39" t="inlineStr">
         <is>
           <t>https://grupaeurocash.pl/assets/media/eurocash-raport-so1-2021-pl.pdf</t>
         </is>
       </c>
-      <c r="S39" t="inlineStr">
+      <c r="V39" t="inlineStr">
         <is>
           <t>Scope 3 nieraportowany</t>
         </is>
       </c>
-      <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
-      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2977,29 +3262,217 @@
         <v>16337</v>
       </c>
       <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr">
+      <c r="P40" t="n">
+        <v>18274</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>108</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1973592</v>
+      </c>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
         <is>
           <t>https://www.citibank.pl/poland/homepage/polish/press1/files/220217-1_ip.pdf</t>
         </is>
       </c>
-      <c r="R40" t="inlineStr">
+      <c r="U40" t="inlineStr">
         <is>
           <t>https://www.citibank.pl/poland/homepage/raport_roczny_2019/files/sprawozdanie_na_temat_informacji_niefinansowych_2019_pl.pdf</t>
         </is>
       </c>
-      <c r="S40" t="inlineStr">
+      <c r="V40" t="inlineStr">
         <is>
           <t>Brak celow dla Scope 3</t>
         </is>
       </c>
-      <c r="T40" t="inlineStr">
+      <c r="W40" t="inlineStr">
         <is>
           <t>Uwzględniane (CO2e)</t>
         </is>
       </c>
-      <c r="U40" t="inlineStr"/>
-      <c r="V40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Millenium Bank</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>25</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K41" t="n">
+        <v>2027</v>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="n">
+        <v>2246</v>
+      </c>
+      <c r="N41" t="n">
+        <v>21434</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="n">
+        <v>23680</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>108</v>
+      </c>
+      <c r="R41" t="n">
+        <v>2557440</v>
+      </c>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Millenium Bank</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>25</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>S1+S2+S3</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="J42" t="n">
+        <v>2020</v>
+      </c>
+      <c r="K42" t="n">
+        <v>2050</v>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="n">
+        <v>2246</v>
+      </c>
+      <c r="N42" t="n">
+        <v>21434</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Grenevia/Famur</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>26</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>S1+S2</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J43" t="n">
+        <v>2021</v>
+      </c>
+      <c r="K43" t="n">
+        <v>2030</v>
+      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="n">
+        <v>1451998</v>
+      </c>
+      <c r="N43" t="n">
+        <v>14236</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="n">
+        <v>1466234</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>28</v>
+      </c>
+      <c r="R43" t="n">
+        <v>41054552</v>
+      </c>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3012,7 +3485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3083,25 +3556,50 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>base_year_ghg_s1s2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>base_year_ghg_s3</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ghg_s3_factor</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ghg_s3_estimate</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>base_year_ghg_s3_estimate</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>company_revenue</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>company_market_cap</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>company_enterprise_value</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>company_total_assets</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>company_cash_equivalents</t>
         </is>
@@ -3136,19 +3634,36 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>11702</v>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>5352870000</v>
+        <v>11124.72</v>
       </c>
       <c r="N2" t="n">
+        <v>206039.04</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>24574.2</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>23361.912</v>
+      </c>
+      <c r="R2" t="n">
+        <v>5352.9</v>
+      </c>
+      <c r="S2" t="n">
         <v>39763.72</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="n">
         <v>16869877000</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3179,19 +3694,34 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>56963</v>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>5638600000</v>
-      </c>
-      <c r="N3" t="n">
+        <v>67960.7</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>119622.3</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>142717.47</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5889.5</v>
+      </c>
+      <c r="S3" t="n">
         <v>5788.57</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="n">
         <v>66647400000</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3222,19 +3752,34 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>5183679</v>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>29803000000</v>
-      </c>
-      <c r="N4" t="n">
+        <v>3045183</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="P4" t="n">
+        <v>13995933.3</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>8221994.1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>31560</v>
+      </c>
+      <c r="S4" t="n">
         <v>27880</v>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="n">
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="n">
         <v>48027000000</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3265,19 +3810,34 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>15945</v>
+      </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>7146633000</v>
-      </c>
-      <c r="N5" t="n">
+        <v>9371.42</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>108</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1722060</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1012113.36</v>
+      </c>
+      <c r="R5" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="S5" t="n">
         <v>18361.13</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="n">
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="n">
         <v>199538885000</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3308,19 +3868,34 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>366700</v>
+      </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>11928000000</v>
-      </c>
-      <c r="N6" t="n">
+        <v>505000</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>770070</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1060500</v>
+      </c>
+      <c r="R6" t="n">
+        <v>12286</v>
+      </c>
+      <c r="S6" t="n">
         <v>11089.42</v>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="n">
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="n">
         <v>26157000000</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3351,19 +3926,34 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>72257</v>
+      </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>9100353000</v>
-      </c>
-      <c r="N7" t="n">
+        <v>72257.39999999999</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
+        <v>108</v>
+      </c>
+      <c r="P7" t="n">
+        <v>7803756</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7803799.2</v>
+      </c>
+      <c r="R7" t="n">
+        <v>8630.030000000001</v>
+      </c>
+      <c r="S7" t="n">
         <v>32021.34</v>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="n">
         <v>250566605000</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3394,19 +3984,34 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>73169805</v>
+      </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>52730000000</v>
-      </c>
-      <c r="N8" t="n">
+        <v>72504413</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P8" t="n">
+        <v>109754707.5</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>108756619.5</v>
+      </c>
+      <c r="R8" t="n">
+        <v>56787</v>
+      </c>
+      <c r="S8" t="n">
         <v>15074.01</v>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="n">
         <v>88966000000</v>
       </c>
-      <c r="Q8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3437,19 +4042,36 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>19237589</v>
+      </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>131341000000</v>
+        <v>18974952</v>
       </c>
       <c r="N9" t="n">
+        <v>81123571</v>
+      </c>
+      <c r="O9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="P9" t="n">
+        <v>144281917.5</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>142312140</v>
+      </c>
+      <c r="R9" t="n">
+        <v>139252</v>
+      </c>
+      <c r="S9" t="n">
         <v>31795.89</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="n">
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="n">
         <v>106754000000</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3480,19 +4102,34 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>50692</v>
+      </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>10568000000</v>
-      </c>
-      <c r="N10" t="n">
+        <v>100722</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
+        <v>108</v>
+      </c>
+      <c r="P10" t="n">
+        <v>5474736</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>10877976</v>
+      </c>
+      <c r="R10" t="n">
+        <v>8384.299999999999</v>
+      </c>
+      <c r="S10" t="n">
         <v>56162.5</v>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
         <v>418086000000</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3523,19 +4160,34 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>126996</v>
+      </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>7454000000</v>
-      </c>
-      <c r="N11" t="n">
+        <v>105583</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="n">
+        <v>108</v>
+      </c>
+      <c r="P11" t="n">
+        <v>13715568</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>11402964</v>
+      </c>
+      <c r="R11" t="n">
+        <v>31335</v>
+      </c>
+      <c r="S11" t="n">
         <v>30525.54</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="n">
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="n">
         <v>402129000000</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3566,19 +4218,34 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>21470</v>
+      </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>9335175000</v>
-      </c>
-      <c r="N12" t="n">
+        <v>9708.219999999999</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="n">
+        <v>108</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2318760</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1048487.76</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4267.36</v>
+      </c>
+      <c r="S12" t="n">
         <v>35612.98</v>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="n">
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="n">
         <v>244876340000</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3609,19 +4276,34 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>2819053</v>
+      </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>3459915000</v>
-      </c>
-      <c r="N13" t="n">
+        <v>3449741</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="P13" t="n">
+        <v>5356200.7</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>6554507.9</v>
+      </c>
+      <c r="R13" t="n">
+        <v>3698.31</v>
+      </c>
+      <c r="S13" t="n">
         <v>2213.4</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="n">
         <v>7145820000</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3652,19 +4334,34 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>22708361</v>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>8018616000</v>
-      </c>
-      <c r="N14" t="n">
+        <v>18671299</v>
+      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P14" t="n">
+        <v>34062541.5</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>28006948.5</v>
+      </c>
+      <c r="R14" t="n">
+        <v>21499.56</v>
+      </c>
+      <c r="S14" t="n">
         <v>3756.68</v>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="n">
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="n">
         <v>34627647000</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3695,19 +4392,34 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="n">
+        <v>3480</v>
+      </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>407571000</v>
-      </c>
-      <c r="N15" t="n">
+        <v>3480.47</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="P15" t="n">
+        <v>7308</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>7308.987</v>
+      </c>
+      <c r="R15" t="n">
+        <v>410.58</v>
+      </c>
+      <c r="S15" t="n">
         <v>1738.48</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="n">
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="n">
         <v>1410688000</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3738,19 +4450,34 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>9328000</v>
+      </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>15901259000</v>
-      </c>
-      <c r="N16" t="n">
+        <v>9362000</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="P16" t="n">
+        <v>17723200</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>17787800</v>
+      </c>
+      <c r="R16" t="n">
+        <v>16</v>
+      </c>
+      <c r="S16" t="n">
         <v>3352.81</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="n">
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="n">
         <v>23644705000</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3781,19 +4508,34 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>8090</v>
+      </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>7757400000</v>
-      </c>
-      <c r="N17" t="n">
+        <v>1511958.27</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="n">
+        <v>108</v>
+      </c>
+      <c r="P17" t="n">
+        <v>873720</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>163291493.2</v>
+      </c>
+      <c r="R17" t="n">
+        <v>8750.5</v>
+      </c>
+      <c r="S17" t="n">
         <v>34736.7</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="n">
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="n">
         <v>201654200000</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3824,19 +4566,34 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>15383718</v>
+      </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>25614000000</v>
-      </c>
-      <c r="N18" t="n">
+        <v>18441041.574</v>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P18" t="n">
+        <v>23075577</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>27661562.36</v>
+      </c>
+      <c r="R18" t="n">
+        <v>25713</v>
+      </c>
+      <c r="S18" t="n">
         <v>4651.27</v>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="n">
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="n">
         <v>40075000000</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3867,19 +4624,34 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>849</v>
+      </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>872239000</v>
-      </c>
-      <c r="N19" t="n">
+        <v>849.4</v>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1782.9</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1783.74</v>
+      </c>
+      <c r="R19" t="n">
+        <v>895.15</v>
+      </c>
+      <c r="S19" t="n">
         <v>4123.71</v>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="n">
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="n">
         <v>1262947000</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3910,19 +4682,34 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>10461</v>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>4705359000</v>
-      </c>
-      <c r="N20" t="n">
+        <v>18984</v>
+      </c>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="n">
+        <v>108</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1129788</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>2050272</v>
+      </c>
+      <c r="R20" t="n">
+        <v>5519.98</v>
+      </c>
+      <c r="S20" t="n">
         <v>13453.71</v>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="n">
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="n">
         <v>131777481000</v>
       </c>
-      <c r="Q20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3953,19 +4740,34 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>3004</v>
+      </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>613972000</v>
-      </c>
-      <c r="N21" t="n">
+        <v>3054.78</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="n">
+        <v>108</v>
+      </c>
+      <c r="P21" t="n">
+        <v>324432</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>329916.24</v>
+      </c>
+      <c r="R21" t="n">
+        <v>652.6799999999999</v>
+      </c>
+      <c r="S21" t="n">
         <v>845.8200000000001</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="n">
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="n">
         <v>20585740000</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3996,19 +4798,34 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="K22" t="n">
+        <v>7920000</v>
+      </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>10629100000</v>
-      </c>
-      <c r="N22" t="n">
+        <v>8220000</v>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="P22" t="n">
+        <v>21384000</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>22194000</v>
+      </c>
+      <c r="R22" t="n">
+        <v>11219.4</v>
+      </c>
+      <c r="S22" t="n">
         <v>4094.14</v>
       </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="n">
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="n">
         <v>15961800000</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -4039,19 +4856,34 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="K23" t="n">
+        <v>186670</v>
+      </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>4794250000</v>
-      </c>
-      <c r="N23" t="n">
+        <v>21123</v>
+      </c>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="n">
+        <v>28</v>
+      </c>
+      <c r="P23" t="n">
+        <v>5226760</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>591444</v>
+      </c>
+      <c r="R23" t="n">
+        <v>4616.27</v>
+      </c>
+      <c r="S23" t="n">
         <v>5886.59</v>
       </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="n">
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="n">
         <v>3526815000</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4082,19 +4914,34 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="n">
+        <v>142429</v>
+      </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>26281431000</v>
-      </c>
-      <c r="N24" t="n">
+        <v>144287.45</v>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="n">
+        <v>10</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1424290</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1442874.5</v>
+      </c>
+      <c r="R24" t="n">
+        <v>26392.16</v>
+      </c>
+      <c r="S24" t="n">
         <v>1508.53</v>
       </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="n">
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="n">
         <v>8487299000</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4125,19 +4972,146 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="n">
+        <v>7758</v>
+      </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>1090108000</v>
-      </c>
-      <c r="N25" t="n">
+        <v>18274</v>
+      </c>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="n">
+        <v>108</v>
+      </c>
+      <c r="P25" t="n">
+        <v>837864</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1973592</v>
+      </c>
+      <c r="R25" t="n">
+        <v>2398.14</v>
+      </c>
+      <c r="S25" t="n">
         <v>7708.92</v>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="n">
         <v>61862771000</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Millenium Bank</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>K6419</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="n">
+        <v>16683</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="n">
+        <v>23680</v>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="n">
+        <v>108</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1801764</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>2557440</v>
+      </c>
+      <c r="R26" t="n">
+        <v>3712.63</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="n">
+        <v>103913000000</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Grenevia/Famur</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>C2824</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="n">
+        <v>1466234</v>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="n">
+        <v>1466234</v>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="n">
+        <v>28</v>
+      </c>
+      <c r="P27" t="n">
+        <v>41054552</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>41054552</v>
+      </c>
+      <c r="R27" t="n">
+        <v>1079</v>
+      </c>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="n">
+        <v>2599000000</v>
+      </c>
+      <c r="V27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4150,7 +5124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4199,7 +5173,9 @@
           <t>LU2237380790</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -4216,7 +5192,9 @@
           <t>PLCCC0000016</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -4233,7 +5211,9 @@
           <t>PLKGHM000017</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -4250,7 +5230,9 @@
           <t>PLBRE0000012</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -4267,7 +5249,9 @@
           <t>PLTLKPL00017</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -4284,7 +5268,9 @@
           <t>PLPEKAO00016</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -4301,7 +5287,9 @@
           <t>PLPGER000010</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -4318,7 +5306,9 @@
           <t>PLPKN0000018</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -4335,7 +5325,9 @@
           <t>PLPKO0000016</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -4352,7 +5344,9 @@
           <t>PLPZU0000011</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
       <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -4369,7 +5363,9 @@
           <t>PLBZ00000044</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -4386,7 +5382,9 @@
           <t>PLCIECH00018</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -4403,7 +5401,9 @@
           <t>PLENEA000013</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -4420,7 +5420,9 @@
           <t>PLGPW0000017</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
       <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -4437,7 +5439,9 @@
           <t>PLZATRM00012</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
       <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -4454,7 +5458,9 @@
           <t>PLBSK0000017</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
       <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -4471,7 +5477,9 @@
           <t>PLTAURN00011</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
       <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -4488,7 +5496,9 @@
           <t>PLWRTPL00027</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
       <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
@@ -4505,7 +5515,9 @@
           <t>PLBGZ0000010</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
       <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -4522,7 +5534,9 @@
           <t>PLBOS0000019</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
       <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -4539,7 +5553,9 @@
           <t>PLJSW0000015</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
       <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -4556,7 +5572,9 @@
           <t>PLKETY000011</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
       <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -4573,7 +5591,9 @@
           <t>PLEURCH00011</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -4590,8 +5610,48 @@
           <t>PLBH00000012</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Millenium Bank</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>PLBIG0000016</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Grenevia/Famur</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PLFAMUR00012</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>